<commit_message>
Update v3.0 template with complete LF Requirements sheet
Regenerated template now includes:
- LF Requirements tab (previously placeholder)
- Examples: Germany, Spain, Malaysia, US, Canada
- Full 22-column structure with global schema

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Country_Rules_Library_v3.0.xlsx
+++ b/Country_Rules_Library_v3.0.xlsx
@@ -9,8 +9,9 @@
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="MF Requirements" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="CbCR Notifications" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TP Forms" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="LF Requirements" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="CbCR Notifications" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="TP Forms" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1792,6 +1793,643 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:V7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="35" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="35" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="35" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
+    <col width="45" customWidth="1" min="21" max="21"/>
+    <col width="45" customWidth="1" min="22" max="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="50" customHeight="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Applicability</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Integrated With</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Submission Channel</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Special Deadline Condition</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Penalty Protection Only</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Rule ID</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Condition Group</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Group Logic</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>Metric Type</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>Metric Scope</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>Threshold Value</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>Operator</t>
+        </is>
+      </c>
+      <c r="O1" s="4" t="inlineStr">
+        <is>
+          <t>Prep Date Rule</t>
+        </is>
+      </c>
+      <c r="P1" s="4" t="inlineStr">
+        <is>
+          <t>Prep Date Details</t>
+        </is>
+      </c>
+      <c r="Q1" s="4" t="inlineStr">
+        <is>
+          <t>Submission Date Rule</t>
+        </is>
+      </c>
+      <c r="R1" s="4" t="inlineStr">
+        <is>
+          <t>Submission Date Details</t>
+        </is>
+      </c>
+      <c r="S1" s="4" t="inlineStr">
+        <is>
+          <t>Upon Request Days</t>
+        </is>
+      </c>
+      <c r="T1" s="4" t="inlineStr">
+        <is>
+          <t>Effective From (FY)</t>
+        </is>
+      </c>
+      <c r="U1" s="4" t="inlineStr">
+        <is>
+          <t>Rule Notes</t>
+        </is>
+      </c>
+      <c r="V1" s="4" t="inlineStr">
+        <is>
+          <t>Deadline Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr"/>
+      <c r="D2" s="5" t="inlineStr"/>
+      <c r="E2" s="5" t="inlineStr"/>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>LF-DE-1</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>RPTs</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t>Transaction (Goods)</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>&gt;</t>
+        </is>
+      </c>
+      <c r="O2" s="5" t="inlineStr">
+        <is>
+          <t>CIT Date</t>
+        </is>
+      </c>
+      <c r="P2" s="5" t="inlineStr">
+        <is>
+          <t>Expected 31 Jul (CIT filing)</t>
+        </is>
+      </c>
+      <c r="Q2" s="5" t="inlineStr">
+        <is>
+          <t>Upon Request</t>
+        </is>
+      </c>
+      <c r="R2" s="5" t="inlineStr">
+        <is>
+          <t>Within 30 days of audit notice</t>
+        </is>
+      </c>
+      <c r="S2" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="T2" s="5" t="inlineStr">
+        <is>
+          <t>FY2024</t>
+        </is>
+      </c>
+      <c r="U2" s="5" t="inlineStr">
+        <is>
+          <t>LF required if goods RPTs exceed 6M EUR</t>
+        </is>
+      </c>
+      <c r="V2" s="5" t="inlineStr">
+        <is>
+          <t>Automatic submission upon audit</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr"/>
+      <c r="D3" s="5" t="inlineStr"/>
+      <c r="E3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>LF-DE-1</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>RPTs</t>
+        </is>
+      </c>
+      <c r="K3" s="5" t="inlineStr">
+        <is>
+          <t>Transaction (Services)</t>
+        </is>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>600000</v>
+      </c>
+      <c r="M3" s="5" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="N3" s="5" t="inlineStr">
+        <is>
+          <t>&gt;</t>
+        </is>
+      </c>
+      <c r="O3" s="5" t="inlineStr">
+        <is>
+          <t>CIT Date</t>
+        </is>
+      </c>
+      <c r="P3" s="5" t="inlineStr">
+        <is>
+          <t>Expected 31 Jul (CIT filing)</t>
+        </is>
+      </c>
+      <c r="Q3" s="5" t="inlineStr">
+        <is>
+          <t>Upon Request</t>
+        </is>
+      </c>
+      <c r="R3" s="5" t="inlineStr">
+        <is>
+          <t>Within 30 days of audit notice</t>
+        </is>
+      </c>
+      <c r="S3" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="T3" s="5" t="inlineStr">
+        <is>
+          <t>FY2024</t>
+        </is>
+      </c>
+      <c r="U3" s="5" t="inlineStr">
+        <is>
+          <t>OR services/other RPTs exceed 600K EUR</t>
+        </is>
+      </c>
+      <c r="V3" s="5" t="inlineStr">
+        <is>
+          <t>Automatic submission upon audit</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr"/>
+      <c r="D4" s="5" t="inlineStr"/>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>LF-ES-1</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>RPTs</t>
+        </is>
+      </c>
+      <c r="K4" s="5" t="inlineStr">
+        <is>
+          <t>Transaction (All)</t>
+        </is>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>250000</v>
+      </c>
+      <c r="M4" s="5" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="N4" s="5" t="inlineStr">
+        <is>
+          <t>&gt;</t>
+        </is>
+      </c>
+      <c r="O4" s="5" t="inlineStr">
+        <is>
+          <t>CIT Date</t>
+        </is>
+      </c>
+      <c r="P4" s="5" t="inlineStr">
+        <is>
+          <t>Expected 25 Jul</t>
+        </is>
+      </c>
+      <c r="Q4" s="5" t="inlineStr">
+        <is>
+          <t>Upon Request</t>
+        </is>
+      </c>
+      <c r="R4" s="5" t="inlineStr">
+        <is>
+          <t>Within 10 days of request</t>
+        </is>
+      </c>
+      <c r="S4" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="T4" s="5" t="inlineStr">
+        <is>
+          <t>FY2016</t>
+        </is>
+      </c>
+      <c r="U4" s="5" t="inlineStr">
+        <is>
+          <t>LF required if local RPTs exceed 250K EUR</t>
+        </is>
+      </c>
+      <c r="V4" s="5" t="inlineStr">
+        <is>
+          <t>Maintain contemporaneously</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Malaysia</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Always</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="5" t="inlineStr"/>
+      <c r="E5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr"/>
+      <c r="H5" s="5" t="inlineStr"/>
+      <c r="I5" s="5" t="inlineStr"/>
+      <c r="J5" s="5" t="inlineStr"/>
+      <c r="K5" s="5" t="inlineStr"/>
+      <c r="L5" s="5" t="inlineStr"/>
+      <c r="M5" s="5" t="inlineStr"/>
+      <c r="N5" s="5" t="inlineStr"/>
+      <c r="O5" s="5" t="inlineStr">
+        <is>
+          <t>CIT Date</t>
+        </is>
+      </c>
+      <c r="P5" s="5" t="inlineStr">
+        <is>
+          <t>By 7 months after FYE (CIT filing)</t>
+        </is>
+      </c>
+      <c r="Q5" s="5" t="inlineStr">
+        <is>
+          <t>Upon Request</t>
+        </is>
+      </c>
+      <c r="R5" s="5" t="inlineStr">
+        <is>
+          <t>Within 14 days</t>
+        </is>
+      </c>
+      <c r="S5" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="T5" s="5" t="inlineStr">
+        <is>
+          <t>FY2023</t>
+        </is>
+      </c>
+      <c r="U5" s="5" t="inlineStr">
+        <is>
+          <t>CTPD (LF) required for all entities with RPTs. MF content integrated per 2023 TPD.</t>
+        </is>
+      </c>
+      <c r="V5" s="5" t="inlineStr">
+        <is>
+          <t>File with CIT return</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr"/>
+      <c r="E6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr"/>
+      <c r="H6" s="5" t="inlineStr"/>
+      <c r="I6" s="5" t="inlineStr"/>
+      <c r="J6" s="5" t="inlineStr"/>
+      <c r="K6" s="5" t="inlineStr"/>
+      <c r="L6" s="5" t="inlineStr"/>
+      <c r="M6" s="5" t="inlineStr"/>
+      <c r="N6" s="5" t="inlineStr"/>
+      <c r="O6" s="5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P6" s="5" t="inlineStr">
+        <is>
+          <t>Voluntary preparation recommended</t>
+        </is>
+      </c>
+      <c r="Q6" s="5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R6" s="5" t="inlineStr">
+        <is>
+          <t>N/A - voluntary</t>
+        </is>
+      </c>
+      <c r="S6" s="5" t="inlineStr"/>
+      <c r="T6" s="5" t="inlineStr">
+        <is>
+          <t>FY2018</t>
+        </is>
+      </c>
+      <c r="U6" s="5" t="inlineStr">
+        <is>
+          <t>Voluntary LF preparation for penalty protection under IRC §6662. No filing requirement.</t>
+        </is>
+      </c>
+      <c r="V6" s="5" t="inlineStr">
+        <is>
+          <t>Contemporaneous documentation provides reasonable cause defense</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="5" t="inlineStr"/>
+      <c r="E7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr"/>
+      <c r="H7" s="5" t="inlineStr"/>
+      <c r="I7" s="5" t="inlineStr"/>
+      <c r="J7" s="5" t="inlineStr"/>
+      <c r="K7" s="5" t="inlineStr"/>
+      <c r="L7" s="5" t="inlineStr"/>
+      <c r="M7" s="5" t="inlineStr"/>
+      <c r="N7" s="5" t="inlineStr"/>
+      <c r="O7" s="5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P7" s="5" t="inlineStr">
+        <is>
+          <t>Voluntary preparation recommended</t>
+        </is>
+      </c>
+      <c r="Q7" s="5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R7" s="5" t="inlineStr">
+        <is>
+          <t>N/A - voluntary</t>
+        </is>
+      </c>
+      <c r="S7" s="5" t="inlineStr"/>
+      <c r="T7" s="5" t="inlineStr">
+        <is>
+          <t>FY2015</t>
+        </is>
+      </c>
+      <c r="U7" s="5" t="inlineStr">
+        <is>
+          <t>Voluntary LF for penalty protection. No statutory filing requirement.</t>
+        </is>
+      </c>
+      <c r="V7" s="5" t="inlineStr">
+        <is>
+          <t>Contemporaneous documentation required for transfer pricing adjustment defense</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2181,7 +2819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Add data validation dropdowns to all sheets
Restored helpful dropdowns from v2.1:
- MF Requirements: 9 dropdown fields (Applicability, Integrated With, Penalty Protection Only, Group Logic, Metric Type, Metric Scope, Operator, Prep/Submission Date Rules)
- LF Requirements: Same 9 dropdown fields
- CbCR Notifications: 7 dropdown fields (Applicability, Frequency, Filer Type, Joint Filing, In CIT, Date Rule, Linked To)
- TP Forms: 6 dropdown fields (Form Type, Trigger, Linked To, Date Rule, E-Signature, Timestamp)

Applied to rows 2-1000 (or 3-1000 for MF/LF with explanation rows)

User feedback: "we also used to have drop downs that were really helpful in the cells to help the user populate"

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Country_Rules_Library_v3.0.xlsx
+++ b/Country_Rules_Library_v3.0.xlsx
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -47,6 +47,10 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="6">
@@ -93,13 +97,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -1248,551 +1255,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-    <col width="45" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="35" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="35" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
-    <col width="35" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
-    <col width="20" customWidth="1" min="20" max="20"/>
-    <col width="45" customWidth="1" min="21" max="21"/>
-    <col width="45" customWidth="1" min="22" max="22"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="50" customHeight="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Country</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Applicability</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Integrated With</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>Submission Channel</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>Special Deadline Condition</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>Penalty Protection Only</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>Rule ID</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>Condition Group</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>Group Logic</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
-        <is>
-          <t>Metric Type</t>
-        </is>
-      </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>Metric Scope</t>
-        </is>
-      </c>
-      <c r="L1" s="4" t="inlineStr">
-        <is>
-          <t>Threshold Value</t>
-        </is>
-      </c>
-      <c r="M1" s="4" t="inlineStr">
-        <is>
-          <t>Currency</t>
-        </is>
-      </c>
-      <c r="N1" s="4" t="inlineStr">
-        <is>
-          <t>Operator</t>
-        </is>
-      </c>
-      <c r="O1" s="4" t="inlineStr">
-        <is>
-          <t>Prep Date Rule</t>
-        </is>
-      </c>
-      <c r="P1" s="4" t="inlineStr">
-        <is>
-          <t>Prep Date Details</t>
-        </is>
-      </c>
-      <c r="Q1" s="4" t="inlineStr">
-        <is>
-          <t>Submission Date Rule</t>
-        </is>
-      </c>
-      <c r="R1" s="4" t="inlineStr">
-        <is>
-          <t>Submission Date Details</t>
-        </is>
-      </c>
-      <c r="S1" s="4" t="inlineStr">
-        <is>
-          <t>Upon Request Days</t>
-        </is>
-      </c>
-      <c r="T1" s="4" t="inlineStr">
-        <is>
-          <t>Effective From (FY)</t>
-        </is>
-      </c>
-      <c r="U1" s="4" t="inlineStr">
-        <is>
-          <t>Rule Notes</t>
-        </is>
-      </c>
-      <c r="V1" s="4" t="inlineStr">
-        <is>
-          <t>Deadline Notes</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>Conditional</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="inlineStr"/>
-      <c r="D2" s="5" t="inlineStr"/>
-      <c r="E2" s="5" t="inlineStr"/>
-      <c r="F2" s="5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr">
-        <is>
-          <t>MF-DE-1</t>
-        </is>
-      </c>
-      <c r="H2" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I2" s="5" t="inlineStr">
-        <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="J2" s="5" t="inlineStr">
-        <is>
-          <t>Revenue</t>
-        </is>
-      </c>
-      <c r="K2" s="5" t="inlineStr">
-        <is>
-          <t>Group (Consolidated)</t>
-        </is>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>750000000</v>
-      </c>
-      <c r="M2" s="5" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="N2" s="5" t="inlineStr">
-        <is>
-          <t>&gt;=</t>
-        </is>
-      </c>
-      <c r="O2" s="5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="P2" s="5" t="inlineStr"/>
-      <c r="Q2" s="5" t="inlineStr">
-        <is>
-          <t>Upon Request</t>
-        </is>
-      </c>
-      <c r="R2" s="5" t="inlineStr">
-        <is>
-          <t>Within 30 days of audit notice</t>
-        </is>
-      </c>
-      <c r="S2" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="T2" s="5" t="inlineStr">
-        <is>
-          <t>FY2024</t>
-        </is>
-      </c>
-      <c r="U2" s="5" t="inlineStr">
-        <is>
-          <t>Standard BEPS threshold</t>
-        </is>
-      </c>
-      <c r="V2" s="5" t="inlineStr">
-        <is>
-          <t>Automatic submission upon audit</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>Conditional</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="inlineStr"/>
-      <c r="D3" s="5" t="inlineStr"/>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>Extraordinary RPTs → full TPD due within 6 months after FYE</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>MF-DE-2</t>
-        </is>
-      </c>
-      <c r="H3" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I3" s="5" t="inlineStr">
-        <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="J3" s="5" t="inlineStr">
-        <is>
-          <t>Always</t>
-        </is>
-      </c>
-      <c r="K3" s="5" t="inlineStr">
-        <is>
-          <t>Local Entity</t>
-        </is>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="N3" s="5" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
-      <c r="O3" s="5" t="inlineStr">
-        <is>
-          <t>FYE-Based</t>
-        </is>
-      </c>
-      <c r="P3" s="5" t="inlineStr">
-        <is>
-          <t>Within 6 months of FYE for extraordinary transactions</t>
-        </is>
-      </c>
-      <c r="Q3" s="5" t="inlineStr">
-        <is>
-          <t>Upon Request</t>
-        </is>
-      </c>
-      <c r="R3" s="5" t="inlineStr">
-        <is>
-          <t>30 days from audit</t>
-        </is>
-      </c>
-      <c r="S3" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="T3" s="5" t="inlineStr">
-        <is>
-          <t>FY2024</t>
-        </is>
-      </c>
-      <c r="U3" s="5" t="inlineStr">
-        <is>
-          <t>Germany-specific extraordinary transaction rule</t>
-        </is>
-      </c>
-      <c r="V3" s="5" t="inlineStr">
-        <is>
-          <t>Separate timeline for extraordinary RPTs</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>Malaysia</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>Integrated</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>Local File</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="inlineStr"/>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr"/>
-      <c r="H4" s="5" t="inlineStr"/>
-      <c r="I4" s="5" t="inlineStr"/>
-      <c r="J4" s="5" t="inlineStr"/>
-      <c r="K4" s="5" t="inlineStr"/>
-      <c r="L4" s="5" t="inlineStr"/>
-      <c r="M4" s="5" t="inlineStr"/>
-      <c r="N4" s="5" t="inlineStr"/>
-      <c r="O4" s="5" t="inlineStr">
-        <is>
-          <t>CIT Date</t>
-        </is>
-      </c>
-      <c r="P4" s="5" t="inlineStr">
-        <is>
-          <t>Prepare with CTPD by CIT filing</t>
-        </is>
-      </c>
-      <c r="Q4" s="5" t="inlineStr">
-        <is>
-          <t>Upon Request</t>
-        </is>
-      </c>
-      <c r="R4" s="5" t="inlineStr">
-        <is>
-          <t>Within 14 days</t>
-        </is>
-      </c>
-      <c r="S4" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="T4" s="5" t="inlineStr">
-        <is>
-          <t>FY2023</t>
-        </is>
-      </c>
-      <c r="U4" s="5" t="inlineStr">
-        <is>
-          <t>MF content integrated into LF per 2023 TPD; no standalone MF. Group revenue below MYR 3B threshold.</t>
-        </is>
-      </c>
-      <c r="V4" s="5" t="inlineStr">
-        <is>
-          <t>MF elements included in CTPD submission</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>Conditional</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="5" t="inlineStr"/>
-      <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr"/>
-      <c r="H5" s="5" t="inlineStr"/>
-      <c r="I5" s="5" t="inlineStr"/>
-      <c r="J5" s="5" t="inlineStr"/>
-      <c r="K5" s="5" t="inlineStr"/>
-      <c r="L5" s="5" t="inlineStr"/>
-      <c r="M5" s="5" t="inlineStr"/>
-      <c r="N5" s="5" t="inlineStr"/>
-      <c r="O5" s="5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="P5" s="5" t="inlineStr">
-        <is>
-          <t>Voluntary preparation recommended</t>
-        </is>
-      </c>
-      <c r="Q5" s="5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="R5" s="5" t="inlineStr">
-        <is>
-          <t>N/A - voluntary</t>
-        </is>
-      </c>
-      <c r="S5" s="5" t="inlineStr"/>
-      <c r="T5" s="5" t="inlineStr">
-        <is>
-          <t>FY2018</t>
-        </is>
-      </c>
-      <c r="U5" s="5" t="inlineStr">
-        <is>
-          <t>Voluntary MF preparation for penalty protection under IRC §6662. No filing requirement.</t>
-        </is>
-      </c>
-      <c r="V5" s="5" t="inlineStr">
-        <is>
-          <t>Contemporaneous documentation provides reasonable cause defense</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>Conditional</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr"/>
-      <c r="H6" s="5" t="inlineStr"/>
-      <c r="I6" s="5" t="inlineStr"/>
-      <c r="J6" s="5" t="inlineStr"/>
-      <c r="K6" s="5" t="inlineStr"/>
-      <c r="L6" s="5" t="inlineStr"/>
-      <c r="M6" s="5" t="inlineStr"/>
-      <c r="N6" s="5" t="inlineStr"/>
-      <c r="O6" s="5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="P6" s="5" t="inlineStr">
-        <is>
-          <t>Voluntary preparation recommended</t>
-        </is>
-      </c>
-      <c r="Q6" s="5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="R6" s="5" t="inlineStr">
-        <is>
-          <t>N/A - voluntary</t>
-        </is>
-      </c>
-      <c r="S6" s="5" t="inlineStr"/>
-      <c r="T6" s="5" t="inlineStr">
-        <is>
-          <t>FY2015</t>
-        </is>
-      </c>
-      <c r="U6" s="5" t="inlineStr">
-        <is>
-          <t>Voluntary MF for penalty protection. No statutory filing requirement.</t>
-        </is>
-      </c>
-      <c r="V6" s="5" t="inlineStr">
-        <is>
-          <t>Contemporaneous documentation required for transfer pricing adjustment defense</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1937,489 +1399,1310 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="60" customHeight="1">
       <c r="A2" s="5" t="inlineStr">
         <is>
+          <t>Germany, Spain, Malaysia, etc.</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Always / Conditional / Integrated / Never Required / N/A</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>Local File / TP Form / Other (only if Integrated)</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>e-filing portal / Form 275.MF / Attachment with CIT / Paper / BZSt Portal</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>Extraordinary RPTs → full TPD due within 6 months after FYE (Germany)</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>Yes / No (US/Canada penalty protection)</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>MF-DE-1, MF-ES-1, etc.</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>1, 2, 3... (increment for multi-conditions)</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>OR / AND (between groups)</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>Revenue / Group Revenue / Employees / RPTs / Balance Sheet / Always / Other</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t>Group (Consolidated) / Local Entity / Transaction (Goods/Services/All)</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>Numeric threshold (e.g., 750000000, 6000000)</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>EUR / USD / GBP / JPY / MYR / etc.</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>&gt;= / &gt; / = / &lt; / &lt;=</t>
+        </is>
+      </c>
+      <c r="O2" s="5" t="inlineStr">
+        <is>
+          <t>None / CIT Date / FYE-Based / Fixed / Upon Request / With Tax Return</t>
+        </is>
+      </c>
+      <c r="P2" s="5" t="inlineStr">
+        <is>
+          <t>Details (e.g., CIT - 5 days, FYE + 10 months, Within 6 months of FYE)</t>
+        </is>
+      </c>
+      <c r="Q2" s="5" t="inlineStr">
+        <is>
+          <t>None / CIT Date / FYE-Based / Fixed / Upon Request / With Tax Return</t>
+        </is>
+      </c>
+      <c r="R2" s="5" t="inlineStr">
+        <is>
+          <t>Details (e.g., 2026-08-25, Within 30 days of audit, By 31 Dec following FY)</t>
+        </is>
+      </c>
+      <c r="S2" s="5" t="inlineStr">
+        <is>
+          <t>Days to submit if upon request (30, 14, 10, etc.)</t>
+        </is>
+      </c>
+      <c r="T2" s="5" t="inlineStr">
+        <is>
+          <t>FY2024, 2023, etc. (when rule took effect)</t>
+        </is>
+      </c>
+      <c r="U2" s="5" t="inlineStr">
+        <is>
+          <t>Threshold rule context and special conditions</t>
+        </is>
+      </c>
+      <c r="V2" s="5" t="inlineStr">
+        <is>
+          <t>Deadline and submission context</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
           <t>Germany</t>
         </is>
       </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr"/>
+      <c r="D3" s="6" t="inlineStr"/>
+      <c r="E3" s="6" t="inlineStr"/>
+      <c r="F3" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="inlineStr">
+        <is>
+          <t>MF-DE-1</t>
+        </is>
+      </c>
+      <c r="H3" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" s="6" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="J3" s="6" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="K3" s="6" t="inlineStr">
+        <is>
+          <t>Group (Consolidated)</t>
+        </is>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>750000000</v>
+      </c>
+      <c r="M3" s="6" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="N3" s="6" t="inlineStr">
+        <is>
+          <t>&gt;=</t>
+        </is>
+      </c>
+      <c r="O3" s="6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P3" s="6" t="inlineStr"/>
+      <c r="Q3" s="6" t="inlineStr">
+        <is>
+          <t>Upon Request</t>
+        </is>
+      </c>
+      <c r="R3" s="6" t="inlineStr">
+        <is>
+          <t>Within 30 days of audit notice</t>
+        </is>
+      </c>
+      <c r="S3" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="T3" s="6" t="inlineStr">
+        <is>
+          <t>FY2024</t>
+        </is>
+      </c>
+      <c r="U3" s="6" t="inlineStr">
+        <is>
+          <t>Standard BEPS threshold</t>
+        </is>
+      </c>
+      <c r="V3" s="6" t="inlineStr">
+        <is>
+          <t>Automatic submission upon audit</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr"/>
+      <c r="D4" s="6" t="inlineStr"/>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>Extraordinary RPTs → full TPD due within 6 months after FYE</t>
+        </is>
+      </c>
+      <c r="F4" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="inlineStr">
+        <is>
+          <t>MF-DE-2</t>
+        </is>
+      </c>
+      <c r="H4" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" s="6" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="J4" s="6" t="inlineStr">
+        <is>
+          <t>Always</t>
+        </is>
+      </c>
+      <c r="K4" s="6" t="inlineStr">
+        <is>
+          <t>Local Entity</t>
+        </is>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="N4" s="6" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="O4" s="6" t="inlineStr">
+        <is>
+          <t>FYE-Based</t>
+        </is>
+      </c>
+      <c r="P4" s="6" t="inlineStr">
+        <is>
+          <t>Within 6 months of FYE for extraordinary transactions</t>
+        </is>
+      </c>
+      <c r="Q4" s="6" t="inlineStr">
+        <is>
+          <t>Upon Request</t>
+        </is>
+      </c>
+      <c r="R4" s="6" t="inlineStr">
+        <is>
+          <t>30 days from audit</t>
+        </is>
+      </c>
+      <c r="S4" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="T4" s="6" t="inlineStr">
+        <is>
+          <t>FY2024</t>
+        </is>
+      </c>
+      <c r="U4" s="6" t="inlineStr">
+        <is>
+          <t>Germany-specific extraordinary transaction rule</t>
+        </is>
+      </c>
+      <c r="V4" s="6" t="inlineStr">
+        <is>
+          <t>Separate timeline for extraordinary RPTs</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Malaysia</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>Local File</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr"/>
+      <c r="E5" s="6" t="inlineStr"/>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="inlineStr"/>
+      <c r="H5" s="6" t="inlineStr"/>
+      <c r="I5" s="6" t="inlineStr"/>
+      <c r="J5" s="6" t="inlineStr"/>
+      <c r="K5" s="6" t="inlineStr"/>
+      <c r="L5" s="6" t="inlineStr"/>
+      <c r="M5" s="6" t="inlineStr"/>
+      <c r="N5" s="6" t="inlineStr"/>
+      <c r="O5" s="6" t="inlineStr">
+        <is>
+          <t>CIT Date</t>
+        </is>
+      </c>
+      <c r="P5" s="6" t="inlineStr">
+        <is>
+          <t>Prepare with CTPD by CIT filing</t>
+        </is>
+      </c>
+      <c r="Q5" s="6" t="inlineStr">
+        <is>
+          <t>Upon Request</t>
+        </is>
+      </c>
+      <c r="R5" s="6" t="inlineStr">
+        <is>
+          <t>Within 14 days</t>
+        </is>
+      </c>
+      <c r="S5" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="T5" s="6" t="inlineStr">
+        <is>
+          <t>FY2023</t>
+        </is>
+      </c>
+      <c r="U5" s="6" t="inlineStr">
+        <is>
+          <t>MF content integrated into LF per 2023 TPD; no standalone MF. Group revenue below MYR 3B threshold.</t>
+        </is>
+      </c>
+      <c r="V5" s="6" t="inlineStr">
+        <is>
+          <t>MF elements included in CTPD submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr"/>
+      <c r="D6" s="6" t="inlineStr"/>
+      <c r="E6" s="6" t="inlineStr"/>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="inlineStr"/>
+      <c r="H6" s="6" t="inlineStr"/>
+      <c r="I6" s="6" t="inlineStr"/>
+      <c r="J6" s="6" t="inlineStr"/>
+      <c r="K6" s="6" t="inlineStr"/>
+      <c r="L6" s="6" t="inlineStr"/>
+      <c r="M6" s="6" t="inlineStr"/>
+      <c r="N6" s="6" t="inlineStr"/>
+      <c r="O6" s="6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P6" s="6" t="inlineStr">
+        <is>
+          <t>Voluntary preparation recommended</t>
+        </is>
+      </c>
+      <c r="Q6" s="6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R6" s="6" t="inlineStr">
+        <is>
+          <t>N/A - voluntary</t>
+        </is>
+      </c>
+      <c r="S6" s="6" t="inlineStr"/>
+      <c r="T6" s="6" t="inlineStr">
+        <is>
+          <t>FY2018</t>
+        </is>
+      </c>
+      <c r="U6" s="6" t="inlineStr">
+        <is>
+          <t>Voluntary MF preparation for penalty protection under IRC §6662. No filing requirement.</t>
+        </is>
+      </c>
+      <c r="V6" s="6" t="inlineStr">
+        <is>
+          <t>Contemporaneous documentation provides reasonable cause defense</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr"/>
+      <c r="D7" s="6" t="inlineStr"/>
+      <c r="E7" s="6" t="inlineStr"/>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G7" s="6" t="inlineStr"/>
+      <c r="H7" s="6" t="inlineStr"/>
+      <c r="I7" s="6" t="inlineStr"/>
+      <c r="J7" s="6" t="inlineStr"/>
+      <c r="K7" s="6" t="inlineStr"/>
+      <c r="L7" s="6" t="inlineStr"/>
+      <c r="M7" s="6" t="inlineStr"/>
+      <c r="N7" s="6" t="inlineStr"/>
+      <c r="O7" s="6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P7" s="6" t="inlineStr">
+        <is>
+          <t>Voluntary preparation recommended</t>
+        </is>
+      </c>
+      <c r="Q7" s="6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R7" s="6" t="inlineStr">
+        <is>
+          <t>N/A - voluntary</t>
+        </is>
+      </c>
+      <c r="S7" s="6" t="inlineStr"/>
+      <c r="T7" s="6" t="inlineStr">
+        <is>
+          <t>FY2015</t>
+        </is>
+      </c>
+      <c r="U7" s="6" t="inlineStr">
+        <is>
+          <t>Voluntary MF for penalty protection. No statutory filing requirement.</t>
+        </is>
+      </c>
+      <c r="V7" s="6" t="inlineStr">
+        <is>
+          <t>Contemporaneous documentation required for transfer pricing adjustment defense</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation sqref="B3:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Always,Conditional,Integrated,Never Required,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Local File,TP Form,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F3:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I3:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AND,OR"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J3:J1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Revenue,Group Revenue,Employees,Balance Sheet,RPTs,Always,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K3:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Group (Consolidated),Local Entity,Transaction (Goods),Transaction (Services),Transaction (All)"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N3:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"&gt;=,&gt;,=,&lt;,&lt;="</formula1>
+    </dataValidation>
+    <dataValidation sqref="O3:O1000 Q3:Q1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"None,CIT Date,FYE-Based,Fixed,Upon Request,With Tax Return"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:V8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="35" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="35" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="35" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
+    <col width="45" customWidth="1" min="21" max="21"/>
+    <col width="45" customWidth="1" min="22" max="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="50" customHeight="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Applicability</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Integrated With</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Submission Channel</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Special Deadline Condition</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Penalty Protection Only</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Rule ID</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Condition Group</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Group Logic</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>Metric Type</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>Metric Scope</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>Threshold Value</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>Operator</t>
+        </is>
+      </c>
+      <c r="O1" s="4" t="inlineStr">
+        <is>
+          <t>Prep Date Rule</t>
+        </is>
+      </c>
+      <c r="P1" s="4" t="inlineStr">
+        <is>
+          <t>Prep Date Details</t>
+        </is>
+      </c>
+      <c r="Q1" s="4" t="inlineStr">
+        <is>
+          <t>Submission Date Rule</t>
+        </is>
+      </c>
+      <c r="R1" s="4" t="inlineStr">
+        <is>
+          <t>Submission Date Details</t>
+        </is>
+      </c>
+      <c r="S1" s="4" t="inlineStr">
+        <is>
+          <t>Upon Request Days</t>
+        </is>
+      </c>
+      <c r="T1" s="4" t="inlineStr">
+        <is>
+          <t>Effective From (FY)</t>
+        </is>
+      </c>
+      <c r="U1" s="4" t="inlineStr">
+        <is>
+          <t>Rule Notes</t>
+        </is>
+      </c>
+      <c r="V1" s="4" t="inlineStr">
+        <is>
+          <t>Deadline Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="60" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Germany, Spain, Malaysia, etc.</t>
+        </is>
+      </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
+          <t>Always / Conditional / Integrated / Never Required / N/A</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>Master File / TP Form / Other (only if Integrated)</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>e-filing portal / With CIT return / Portal / Paper</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>Extraordinary RPTs → full TPD due within 6 months after FYE (Germany)</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>Yes / No (US/Canada penalty protection)</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>LF-DE-1, LF-ES-1, etc.</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>1, 2, 3... (increment for multi-conditions)</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>OR / AND (between groups)</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>Revenue / Group Revenue / Employees / RPTs / Balance Sheet / Always / Other</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t>Group (Consolidated) / Local Entity / Transaction (Goods/Services/All)</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>Numeric threshold (e.g., 6000000, 250000)</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>EUR / USD / GBP / JPY / MYR / etc.</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>&gt;= / &gt; / = / &lt; / &lt;=</t>
+        </is>
+      </c>
+      <c r="O2" s="5" t="inlineStr">
+        <is>
+          <t>None / CIT Date / FYE-Based / Fixed / Upon Request / With Tax Return</t>
+        </is>
+      </c>
+      <c r="P2" s="5" t="inlineStr">
+        <is>
+          <t>Details (e.g., Expected 31 Jul, By 7 months after FYE)</t>
+        </is>
+      </c>
+      <c r="Q2" s="5" t="inlineStr">
+        <is>
+          <t>None / CIT Date / FYE-Based / Fixed / Upon Request / With Tax Return</t>
+        </is>
+      </c>
+      <c r="R2" s="5" t="inlineStr">
+        <is>
+          <t>Details (e.g., Within 30 days of audit, Within 10 days of request)</t>
+        </is>
+      </c>
+      <c r="S2" s="5" t="inlineStr">
+        <is>
+          <t>Days to submit if upon request (30, 14, 10, etc.)</t>
+        </is>
+      </c>
+      <c r="T2" s="5" t="inlineStr">
+        <is>
+          <t>FY2024, 2023, etc. (when rule took effect)</t>
+        </is>
+      </c>
+      <c r="U2" s="5" t="inlineStr">
+        <is>
+          <t>Threshold rule context and special conditions</t>
+        </is>
+      </c>
+      <c r="V2" s="5" t="inlineStr">
+        <is>
+          <t>Deadline and submission context</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr"/>
-      <c r="D2" s="5" t="inlineStr"/>
-      <c r="E2" s="5" t="inlineStr"/>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr"/>
+      <c r="D3" s="6" t="inlineStr"/>
+      <c r="E3" s="6" t="inlineStr"/>
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>LF-DE-1</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H3" s="6" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I3" s="6" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="J3" s="6" t="inlineStr">
         <is>
           <t>RPTs</t>
         </is>
       </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="K3" s="6" t="inlineStr">
         <is>
           <t>Transaction (Goods)</t>
         </is>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L3" s="6" t="n">
         <v>6000000</v>
       </c>
-      <c r="M2" s="5" t="inlineStr">
+      <c r="M3" s="6" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="N3" s="6" t="inlineStr">
         <is>
           <t>&gt;</t>
         </is>
       </c>
-      <c r="O2" s="5" t="inlineStr">
+      <c r="O3" s="6" t="inlineStr">
         <is>
           <t>CIT Date</t>
         </is>
       </c>
-      <c r="P2" s="5" t="inlineStr">
+      <c r="P3" s="6" t="inlineStr">
         <is>
           <t>Expected 31 Jul (CIT filing)</t>
         </is>
       </c>
-      <c r="Q2" s="5" t="inlineStr">
+      <c r="Q3" s="6" t="inlineStr">
         <is>
           <t>Upon Request</t>
         </is>
       </c>
-      <c r="R2" s="5" t="inlineStr">
+      <c r="R3" s="6" t="inlineStr">
         <is>
           <t>Within 30 days of audit notice</t>
         </is>
       </c>
-      <c r="S2" s="5" t="n">
+      <c r="S3" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="T2" s="5" t="inlineStr">
+      <c r="T3" s="6" t="inlineStr">
         <is>
           <t>FY2024</t>
         </is>
       </c>
-      <c r="U2" s="5" t="inlineStr">
+      <c r="U3" s="6" t="inlineStr">
         <is>
           <t>LF required if goods RPTs exceed 6M EUR</t>
         </is>
       </c>
-      <c r="V2" s="5" t="inlineStr">
+      <c r="V3" s="6" t="inlineStr">
         <is>
           <t>Automatic submission upon audit</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Germany</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr"/>
-      <c r="D3" s="5" t="inlineStr"/>
-      <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr"/>
+      <c r="D4" s="6" t="inlineStr"/>
+      <c r="E4" s="6" t="inlineStr"/>
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>LF-DE-1</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="H4" s="6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="I4" s="6" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="J4" s="6" t="inlineStr">
         <is>
           <t>RPTs</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="K4" s="6" t="inlineStr">
         <is>
           <t>Transaction (Services)</t>
         </is>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L4" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="M3" s="5" t="inlineStr">
+      <c r="M4" s="6" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="N3" s="5" t="inlineStr">
+      <c r="N4" s="6" t="inlineStr">
         <is>
           <t>&gt;</t>
         </is>
       </c>
-      <c r="O3" s="5" t="inlineStr">
+      <c r="O4" s="6" t="inlineStr">
         <is>
           <t>CIT Date</t>
         </is>
       </c>
-      <c r="P3" s="5" t="inlineStr">
+      <c r="P4" s="6" t="inlineStr">
         <is>
           <t>Expected 31 Jul (CIT filing)</t>
         </is>
       </c>
-      <c r="Q3" s="5" t="inlineStr">
+      <c r="Q4" s="6" t="inlineStr">
         <is>
           <t>Upon Request</t>
         </is>
       </c>
-      <c r="R3" s="5" t="inlineStr">
+      <c r="R4" s="6" t="inlineStr">
         <is>
           <t>Within 30 days of audit notice</t>
         </is>
       </c>
-      <c r="S3" s="5" t="n">
+      <c r="S4" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="T3" s="5" t="inlineStr">
+      <c r="T4" s="6" t="inlineStr">
         <is>
           <t>FY2024</t>
         </is>
       </c>
-      <c r="U3" s="5" t="inlineStr">
+      <c r="U4" s="6" t="inlineStr">
         <is>
           <t>OR services/other RPTs exceed 600K EUR</t>
         </is>
       </c>
-      <c r="V3" s="5" t="inlineStr">
+      <c r="V4" s="6" t="inlineStr">
         <is>
           <t>Automatic submission upon audit</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="5" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Spain</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="5" t="inlineStr"/>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr"/>
+      <c r="D5" s="6" t="inlineStr"/>
+      <c r="E5" s="6" t="inlineStr"/>
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>LF-ES-1</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="H5" s="6" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="I5" s="6" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
       </c>
-      <c r="J4" s="5" t="inlineStr">
+      <c r="J5" s="6" t="inlineStr">
         <is>
           <t>RPTs</t>
         </is>
       </c>
-      <c r="K4" s="5" t="inlineStr">
+      <c r="K5" s="6" t="inlineStr">
         <is>
           <t>Transaction (All)</t>
         </is>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L5" s="6" t="n">
         <v>250000</v>
       </c>
-      <c r="M4" s="5" t="inlineStr">
+      <c r="M5" s="6" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="N4" s="5" t="inlineStr">
+      <c r="N5" s="6" t="inlineStr">
         <is>
           <t>&gt;</t>
         </is>
       </c>
-      <c r="O4" s="5" t="inlineStr">
+      <c r="O5" s="6" t="inlineStr">
         <is>
           <t>CIT Date</t>
         </is>
       </c>
-      <c r="P4" s="5" t="inlineStr">
+      <c r="P5" s="6" t="inlineStr">
         <is>
           <t>Expected 25 Jul</t>
         </is>
       </c>
-      <c r="Q4" s="5" t="inlineStr">
+      <c r="Q5" s="6" t="inlineStr">
         <is>
           <t>Upon Request</t>
         </is>
       </c>
-      <c r="R4" s="5" t="inlineStr">
+      <c r="R5" s="6" t="inlineStr">
         <is>
           <t>Within 10 days of request</t>
         </is>
       </c>
-      <c r="S4" s="5" t="n">
+      <c r="S5" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="T4" s="5" t="inlineStr">
+      <c r="T5" s="6" t="inlineStr">
         <is>
           <t>FY2016</t>
         </is>
       </c>
-      <c r="U4" s="5" t="inlineStr">
+      <c r="U5" s="6" t="inlineStr">
         <is>
           <t>LF required if local RPTs exceed 250K EUR</t>
         </is>
       </c>
-      <c r="V4" s="5" t="inlineStr">
+      <c r="V5" s="6" t="inlineStr">
         <is>
           <t>Maintain contemporaneously</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>Malaysia</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Always</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="5" t="inlineStr"/>
-      <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr"/>
+      <c r="D6" s="6" t="inlineStr"/>
+      <c r="E6" s="6" t="inlineStr"/>
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G5" s="5" t="inlineStr"/>
-      <c r="H5" s="5" t="inlineStr"/>
-      <c r="I5" s="5" t="inlineStr"/>
-      <c r="J5" s="5" t="inlineStr"/>
-      <c r="K5" s="5" t="inlineStr"/>
-      <c r="L5" s="5" t="inlineStr"/>
-      <c r="M5" s="5" t="inlineStr"/>
-      <c r="N5" s="5" t="inlineStr"/>
-      <c r="O5" s="5" t="inlineStr">
+      <c r="G6" s="6" t="inlineStr"/>
+      <c r="H6" s="6" t="inlineStr"/>
+      <c r="I6" s="6" t="inlineStr"/>
+      <c r="J6" s="6" t="inlineStr"/>
+      <c r="K6" s="6" t="inlineStr"/>
+      <c r="L6" s="6" t="inlineStr"/>
+      <c r="M6" s="6" t="inlineStr"/>
+      <c r="N6" s="6" t="inlineStr"/>
+      <c r="O6" s="6" t="inlineStr">
         <is>
           <t>CIT Date</t>
         </is>
       </c>
-      <c r="P5" s="5" t="inlineStr">
+      <c r="P6" s="6" t="inlineStr">
         <is>
           <t>By 7 months after FYE (CIT filing)</t>
         </is>
       </c>
-      <c r="Q5" s="5" t="inlineStr">
+      <c r="Q6" s="6" t="inlineStr">
         <is>
           <t>Upon Request</t>
         </is>
       </c>
-      <c r="R5" s="5" t="inlineStr">
+      <c r="R6" s="6" t="inlineStr">
         <is>
           <t>Within 14 days</t>
         </is>
       </c>
-      <c r="S5" s="5" t="n">
+      <c r="S6" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="T5" s="5" t="inlineStr">
+      <c r="T6" s="6" t="inlineStr">
         <is>
           <t>FY2023</t>
         </is>
       </c>
-      <c r="U5" s="5" t="inlineStr">
+      <c r="U6" s="6" t="inlineStr">
         <is>
           <t>CTPD (LF) required for all entities with RPTs. MF content integrated per 2023 TPD.</t>
         </is>
       </c>
-      <c r="V5" s="5" t="inlineStr">
+      <c r="V6" s="6" t="inlineStr">
         <is>
           <t>File with CIT return</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="5" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr"/>
+      <c r="D7" s="6" t="inlineStr"/>
+      <c r="E7" s="6" t="inlineStr"/>
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G6" s="5" t="inlineStr"/>
-      <c r="H6" s="5" t="inlineStr"/>
-      <c r="I6" s="5" t="inlineStr"/>
-      <c r="J6" s="5" t="inlineStr"/>
-      <c r="K6" s="5" t="inlineStr"/>
-      <c r="L6" s="5" t="inlineStr"/>
-      <c r="M6" s="5" t="inlineStr"/>
-      <c r="N6" s="5" t="inlineStr"/>
-      <c r="O6" s="5" t="inlineStr">
+      <c r="G7" s="6" t="inlineStr"/>
+      <c r="H7" s="6" t="inlineStr"/>
+      <c r="I7" s="6" t="inlineStr"/>
+      <c r="J7" s="6" t="inlineStr"/>
+      <c r="K7" s="6" t="inlineStr"/>
+      <c r="L7" s="6" t="inlineStr"/>
+      <c r="M7" s="6" t="inlineStr"/>
+      <c r="N7" s="6" t="inlineStr"/>
+      <c r="O7" s="6" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="P6" s="5" t="inlineStr">
+      <c r="P7" s="6" t="inlineStr">
         <is>
           <t>Voluntary preparation recommended</t>
         </is>
       </c>
-      <c r="Q6" s="5" t="inlineStr">
+      <c r="Q7" s="6" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="R6" s="5" t="inlineStr">
+      <c r="R7" s="6" t="inlineStr">
         <is>
           <t>N/A - voluntary</t>
         </is>
       </c>
-      <c r="S6" s="5" t="inlineStr"/>
-      <c r="T6" s="5" t="inlineStr">
+      <c r="S7" s="6" t="inlineStr"/>
+      <c r="T7" s="6" t="inlineStr">
         <is>
           <t>FY2018</t>
         </is>
       </c>
-      <c r="U6" s="5" t="inlineStr">
+      <c r="U7" s="6" t="inlineStr">
         <is>
           <t>Voluntary LF preparation for penalty protection under IRC §6662. No filing requirement.</t>
         </is>
       </c>
-      <c r="V6" s="5" t="inlineStr">
+      <c r="V7" s="6" t="inlineStr">
         <is>
           <t>Contemporaneous documentation provides reasonable cause defense</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="5" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="5" t="inlineStr"/>
-      <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr"/>
+      <c r="D8" s="6" t="inlineStr"/>
+      <c r="E8" s="6" t="inlineStr"/>
+      <c r="F8" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G7" s="5" t="inlineStr"/>
-      <c r="H7" s="5" t="inlineStr"/>
-      <c r="I7" s="5" t="inlineStr"/>
-      <c r="J7" s="5" t="inlineStr"/>
-      <c r="K7" s="5" t="inlineStr"/>
-      <c r="L7" s="5" t="inlineStr"/>
-      <c r="M7" s="5" t="inlineStr"/>
-      <c r="N7" s="5" t="inlineStr"/>
-      <c r="O7" s="5" t="inlineStr">
+      <c r="G8" s="6" t="inlineStr"/>
+      <c r="H8" s="6" t="inlineStr"/>
+      <c r="I8" s="6" t="inlineStr"/>
+      <c r="J8" s="6" t="inlineStr"/>
+      <c r="K8" s="6" t="inlineStr"/>
+      <c r="L8" s="6" t="inlineStr"/>
+      <c r="M8" s="6" t="inlineStr"/>
+      <c r="N8" s="6" t="inlineStr"/>
+      <c r="O8" s="6" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="P7" s="5" t="inlineStr">
+      <c r="P8" s="6" t="inlineStr">
         <is>
           <t>Voluntary preparation recommended</t>
         </is>
       </c>
-      <c r="Q7" s="5" t="inlineStr">
+      <c r="Q8" s="6" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="R7" s="5" t="inlineStr">
+      <c r="R8" s="6" t="inlineStr">
         <is>
           <t>N/A - voluntary</t>
         </is>
       </c>
-      <c r="S7" s="5" t="inlineStr"/>
-      <c r="T7" s="5" t="inlineStr">
+      <c r="S8" s="6" t="inlineStr"/>
+      <c r="T8" s="6" t="inlineStr">
         <is>
           <t>FY2015</t>
         </is>
       </c>
-      <c r="U7" s="5" t="inlineStr">
+      <c r="U8" s="6" t="inlineStr">
         <is>
           <t>Voluntary LF for penalty protection. No statutory filing requirement.</t>
         </is>
       </c>
-      <c r="V7" s="5" t="inlineStr">
+      <c r="V8" s="6" t="inlineStr">
         <is>
           <t>Contemporaneous documentation required for transfer pricing adjustment defense</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="8">
+    <dataValidation sqref="B3:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Always,Conditional,Integrated,Never Required,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Master File,TP Form,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F3:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I3:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AND,OR"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J3:J1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Revenue,Group Revenue,Employees,Balance Sheet,RPTs,Always,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K3:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Group (Consolidated),Local Entity,Transaction (Goods),Transaction (Services),Transaction (All)"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N3:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"&gt;=,&gt;,=,&lt;,&lt;="</formula1>
+    </dataValidation>
+    <dataValidation sqref="O3:O1000 Q3:Q1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"None,CIT Date,FYE-Based,Fixed,Upon Request,With Tax Return"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2527,294 +2810,317 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Belgium</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>Annual</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
         <is>
           <t>Local CE</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Separate Form</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H2" s="6" t="inlineStr">
         <is>
           <t>Form 275.CBC.NOT</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I2" s="6" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="J2" s="6" t="inlineStr">
         <is>
           <t>By 31 Dec following FY</t>
         </is>
       </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="K2" s="6" t="inlineStr">
         <is>
           <t>Valid for FY</t>
         </is>
       </c>
-      <c r="L2" s="5" t="inlineStr">
+      <c r="L2" s="6" t="inlineStr">
         <is>
           <t>CbCR</t>
         </is>
       </c>
-      <c r="M2" s="5" t="inlineStr">
+      <c r="M2" s="6" t="inlineStr">
         <is>
           <t>FY2016</t>
         </is>
       </c>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="N2" s="6" t="inlineStr">
         <is>
           <t>Annual CbCR notification filed separately from CIT return</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>France</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>Upon Change</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
         <is>
           <t>UPE</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>Not Specified</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>Portal</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="H3" s="6" t="inlineStr">
         <is>
           <t>DAS2-CbCR</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="I3" s="6" t="inlineStr">
         <is>
           <t>Upon Change</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="J3" s="6" t="inlineStr">
         <is>
           <t>Within 3 months of change</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="K3" s="6" t="inlineStr">
         <is>
           <t>Until entity or UPE info changes</t>
         </is>
       </c>
-      <c r="L3" s="5" t="inlineStr">
+      <c r="L3" s="6" t="inlineStr">
         <is>
           <t>CbCR</t>
         </is>
       </c>
-      <c r="M3" s="5" t="inlineStr">
+      <c r="M3" s="6" t="inlineStr">
         <is>
           <t>FY2017</t>
         </is>
       </c>
-      <c r="N3" s="5" t="inlineStr">
+      <c r="N3" s="6" t="inlineStr">
         <is>
           <t>One-time notification valid until circumstances change (UPE change, threshold, etc.)</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>Upon Change</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
         <is>
           <t>UPE</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>Not Specified</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Within CIT Return</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="H4" s="6" t="inlineStr">
         <is>
           <t>SA</t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="I4" s="6" t="inlineStr">
         <is>
           <t>With Tax Return</t>
         </is>
       </c>
-      <c r="J4" s="5" t="inlineStr">
+      <c r="J4" s="6" t="inlineStr">
         <is>
           <t>Within CIT return filing</t>
         </is>
       </c>
-      <c r="K4" s="5" t="inlineStr">
+      <c r="K4" s="6" t="inlineStr">
         <is>
           <t>Until change in filing entity</t>
         </is>
       </c>
-      <c r="L4" s="5" t="inlineStr">
+      <c r="L4" s="6" t="inlineStr">
         <is>
           <t>CbCR</t>
         </is>
       </c>
-      <c r="M4" s="5" t="inlineStr">
+      <c r="M4" s="6" t="inlineStr">
         <is>
           <t>FY2016</t>
         </is>
       </c>
-      <c r="N4" s="5" t="inlineStr">
+      <c r="N4" s="6" t="inlineStr">
         <is>
           <t>Notification included in CIT return; updated when filing entity changes</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Germany</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>Annual</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>One CE for All</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>BZSt Portal</t>
         </is>
       </c>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="H5" s="6" t="inlineStr">
         <is>
           <t>BZSt CbCR Notification</t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr">
+      <c r="I5" s="6" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="J5" s="5" t="inlineStr">
+      <c r="J5" s="6" t="inlineStr">
         <is>
           <t>By end of reporting FY</t>
         </is>
       </c>
-      <c r="K5" s="5" t="inlineStr">
+      <c r="K5" s="6" t="inlineStr">
         <is>
           <t>Annual</t>
         </is>
       </c>
-      <c r="L5" s="5" t="inlineStr">
+      <c r="L5" s="6" t="inlineStr">
         <is>
           <t>CbCR</t>
         </is>
       </c>
-      <c r="M5" s="5" t="inlineStr">
+      <c r="M5" s="6" t="inlineStr">
         <is>
           <t>FY2016</t>
         </is>
       </c>
-      <c r="N5" s="5" t="inlineStr">
+      <c r="N5" s="6" t="inlineStr">
         <is>
           <t>One German group entity can file notification for all German entities</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="7">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Always,Conditional,Notification Only,Never Required,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Annual,One-Time,Upon Change"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"UPE,Local CE,One CE for All,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Yes,No,Not Specified"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"None,CIT Date,FYE-Based,Fixed,Upon Request,With Tax Return"</formula1>
+    </dataValidation>
+    <dataValidation sqref="L2:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"MF,LF,CbCR,Standalone"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2916,323 +3222,343 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Belgium</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Form 275.MF</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>MF Summary</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
         <is>
           <t>If MF Required</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>MF</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>Summary form with key MF data points</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H2" s="6" t="inlineStr">
         <is>
           <t>31 Dec following FY</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr"/>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="I2" s="6" t="inlineStr"/>
+      <c r="J2" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="K2" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="L2" s="5" t="inlineStr">
+      <c r="L2" s="6" t="inlineStr">
         <is>
           <t>FY2016</t>
         </is>
       </c>
-      <c r="M2" s="5" t="inlineStr">
+      <c r="M2" s="6" t="inlineStr">
         <is>
           <t>Separate summary form filed alongside full MF report</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Belgium</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>Form 275.LF</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>LF Summary</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
         <is>
           <t>If LF Required</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>LF</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>Summary form with key LF data points</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>With Tax Return</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="H3" s="6" t="inlineStr">
         <is>
           <t>Expected 31 Jul</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr"/>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="I3" s="6" t="inlineStr"/>
+      <c r="J3" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="K3" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="L3" s="5" t="inlineStr">
+      <c r="L3" s="6" t="inlineStr">
         <is>
           <t>FY2016</t>
         </is>
       </c>
-      <c r="M3" s="5" t="inlineStr">
+      <c r="M3" s="6" t="inlineStr">
         <is>
           <t>Separate summary form filed with CIT return</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Spain</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Form 232</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>TP Return</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
         <is>
           <t>If MF or LF Required</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>Standalone</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>Annual TP informative return</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="H4" s="6" t="inlineStr">
         <is>
           <t>Approx 25 Aug</t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr"/>
-      <c r="J4" s="5" t="inlineStr">
+      <c r="I4" s="6" t="inlineStr"/>
+      <c r="J4" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K4" s="5" t="inlineStr">
+      <c r="K4" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="L4" s="5" t="inlineStr">
+      <c r="L4" s="6" t="inlineStr">
         <is>
           <t>FY2016</t>
         </is>
       </c>
-      <c r="M4" s="5" t="inlineStr">
+      <c r="M4" s="6" t="inlineStr">
         <is>
           <t>Informative return separate from full MF/LF documentation</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>RS 106</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>TP Disclosure</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>If MF or LF Required</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>Standalone</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>TP disclosure in tax return</t>
         </is>
       </c>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>With Tax Return</t>
         </is>
       </c>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="H5" s="6" t="inlineStr">
         <is>
           <t>Expected 31 Oct</t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr"/>
-      <c r="J5" s="5" t="inlineStr">
+      <c r="I5" s="6" t="inlineStr"/>
+      <c r="J5" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K5" s="5" t="inlineStr">
+      <c r="K5" s="6" t="inlineStr">
         <is>
           <t>Electronic Timestamp</t>
         </is>
       </c>
-      <c r="L5" s="5" t="inlineStr">
+      <c r="L5" s="6" t="inlineStr">
         <is>
           <t>FY2010</t>
         </is>
       </c>
-      <c r="M5" s="5" t="inlineStr">
+      <c r="M5" s="6" t="inlineStr">
         <is>
           <t>MF/LF must be electronically timestamped before filing RS 106 disclosure</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="inlineStr">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>Germany</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Transaction Matrix</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>TP Disclosure</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D6" s="6" t="inlineStr">
         <is>
           <t>Always</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>MF</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>Structured overview of RPTs</t>
         </is>
       </c>
-      <c r="G6" s="5" t="inlineStr">
+      <c r="G6" s="6" t="inlineStr">
         <is>
           <t>Upon Request</t>
         </is>
       </c>
-      <c r="H6" s="5" t="inlineStr">
+      <c r="H6" s="6" t="inlineStr">
         <is>
           <t>Within 30 days of audit notice</t>
         </is>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="J6" s="5" t="inlineStr">
+      <c r="J6" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K6" s="5" t="inlineStr">
+      <c r="K6" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L6" s="5" t="inlineStr">
+      <c r="L6" s="6" t="inlineStr">
         <is>
           <t>FY2024</t>
         </is>
       </c>
-      <c r="M6" s="5" t="inlineStr">
+      <c r="M6" s="6" t="inlineStr">
         <is>
           <t>NEW 2024 requirement - automatic submission with MF upon audit</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"TP Disclosure,TP Return,MF Summary,LF Summary,CbCR Notification,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Always,If MF Required,If LF Required,If MF or LF Required,If CbCR Required,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"MF,LF,CbCR,Standalone"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"None,CIT Date,FYE-Based,Fixed,Upon Request,With Tax Return"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Yes,No,Electronic Timestamp"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add explanation rows to CbCR Notifications and TP Forms sheets
Completed explanation rows for all sheets:
- CbCR Notifications: 14-column explanation row with examples
- TP Forms: 13-column explanation row with examples
- Updated example data to start from row 3 (row 2 = explanations)
- Fixed dropdown validations to apply from row 3-1000

All 4 main sheets now have:
- Row 1: Headers (dark blue)
- Row 2: Explanations (yellow, italic)
- Row 3+: Data/examples (green)

User feedback: "you didnt put in the explanation row in each tab"

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Country_Rules_Library_v3.0.xlsx
+++ b/Country_Rules_Library_v3.0.xlsx
@@ -2713,7 +2713,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2809,82 +2809,82 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="6" t="inlineStr">
-        <is>
-          <t>Belgium</t>
-        </is>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Conditional</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>Annual</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
-        <is>
-          <t>Local CE</t>
-        </is>
-      </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F2" s="6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G2" s="6" t="inlineStr">
-        <is>
-          <t>Separate Form</t>
-        </is>
-      </c>
-      <c r="H2" s="6" t="inlineStr">
-        <is>
-          <t>Form 275.CBC.NOT</t>
-        </is>
-      </c>
-      <c r="I2" s="6" t="inlineStr">
-        <is>
-          <t>Fixed</t>
-        </is>
-      </c>
-      <c r="J2" s="6" t="inlineStr">
-        <is>
-          <t>By 31 Dec following FY</t>
-        </is>
-      </c>
-      <c r="K2" s="6" t="inlineStr">
-        <is>
-          <t>Valid for FY</t>
-        </is>
-      </c>
-      <c r="L2" s="6" t="inlineStr">
-        <is>
-          <t>CbCR</t>
-        </is>
-      </c>
-      <c r="M2" s="6" t="inlineStr">
-        <is>
-          <t>FY2016</t>
-        </is>
-      </c>
-      <c r="N2" s="6" t="inlineStr">
-        <is>
-          <t>Annual CbCR notification filed separately from CIT return</t>
+    <row r="2" ht="60" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Belgium, France, UK, Germany, etc.</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Always / Conditional / Notification Only / Never Required / N/A</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>Annual / One-Time / Upon Change</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>UPE / Local CE / One CE for All / Other</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>Yes / No / Not Specified</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>Yes / No</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>Separate Form / Portal / Within CIT Return / BZSt Portal</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>Form 275.CBC.NOT / DAS2-CbCR / SA / BZSt CbCR Notification</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>None / CIT Date / FYE-Based / Fixed / Upon Request / With Tax Return</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>Details (e.g., By 31 Dec following FY, Within 3 months of change)</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t>Valid for FY / Until entity or UPE info changes / Annual / Until change in filing entity</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>MF / LF / CbCR / Standalone</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>FY2016, 2017, etc.</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>Context about notification rules and requirements</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="B3" s="6" t="inlineStr">
@@ -2894,17 +2894,17 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Upon Change</t>
+          <t>Annual</t>
         </is>
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>UPE</t>
+          <t>Local CE</t>
         </is>
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F3" s="6" t="inlineStr">
@@ -2914,27 +2914,27 @@
       </c>
       <c r="G3" s="6" t="inlineStr">
         <is>
-          <t>Portal</t>
+          <t>Separate Form</t>
         </is>
       </c>
       <c r="H3" s="6" t="inlineStr">
         <is>
-          <t>DAS2-CbCR</t>
+          <t>Form 275.CBC.NOT</t>
         </is>
       </c>
       <c r="I3" s="6" t="inlineStr">
         <is>
-          <t>Upon Change</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="J3" s="6" t="inlineStr">
         <is>
-          <t>Within 3 months of change</t>
+          <t>By 31 Dec following FY</t>
         </is>
       </c>
       <c r="K3" s="6" t="inlineStr">
         <is>
-          <t>Until entity or UPE info changes</t>
+          <t>Valid for FY</t>
         </is>
       </c>
       <c r="L3" s="6" t="inlineStr">
@@ -2944,19 +2944,19 @@
       </c>
       <c r="M3" s="6" t="inlineStr">
         <is>
-          <t>FY2017</t>
+          <t>FY2016</t>
         </is>
       </c>
       <c r="N3" s="6" t="inlineStr">
         <is>
-          <t>One-time notification valid until circumstances change (UPE change, threshold, etc.)</t>
+          <t>Annual CbCR notification filed separately from CIT return</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>France</t>
         </is>
       </c>
       <c r="B4" s="6" t="inlineStr">
@@ -2981,32 +2981,32 @@
       </c>
       <c r="F4" s="6" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
-          <t>Within CIT Return</t>
+          <t>Portal</t>
         </is>
       </c>
       <c r="H4" s="6" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>DAS2-CbCR</t>
         </is>
       </c>
       <c r="I4" s="6" t="inlineStr">
         <is>
-          <t>With Tax Return</t>
+          <t>Upon Change</t>
         </is>
       </c>
       <c r="J4" s="6" t="inlineStr">
         <is>
-          <t>Within CIT return filing</t>
+          <t>Within 3 months of change</t>
         </is>
       </c>
       <c r="K4" s="6" t="inlineStr">
         <is>
-          <t>Until change in filing entity</t>
+          <t>Until entity or UPE info changes</t>
         </is>
       </c>
       <c r="L4" s="6" t="inlineStr">
@@ -3016,82 +3016,154 @@
       </c>
       <c r="M4" s="6" t="inlineStr">
         <is>
-          <t>FY2016</t>
+          <t>FY2017</t>
         </is>
       </c>
       <c r="N4" s="6" t="inlineStr">
         <is>
-          <t>Notification included in CIT return; updated when filing entity changes</t>
+          <t>One-time notification valid until circumstances change (UPE change, threshold, etc.)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>Upon Change</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>UPE</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>Not Specified</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="inlineStr">
+        <is>
+          <t>Within CIT Return</t>
+        </is>
+      </c>
+      <c r="H5" s="6" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="I5" s="6" t="inlineStr">
+        <is>
+          <t>With Tax Return</t>
+        </is>
+      </c>
+      <c r="J5" s="6" t="inlineStr">
+        <is>
+          <t>Within CIT return filing</t>
+        </is>
+      </c>
+      <c r="K5" s="6" t="inlineStr">
+        <is>
+          <t>Until change in filing entity</t>
+        </is>
+      </c>
+      <c r="L5" s="6" t="inlineStr">
+        <is>
+          <t>CbCR</t>
+        </is>
+      </c>
+      <c r="M5" s="6" t="inlineStr">
+        <is>
+          <t>FY2016</t>
+        </is>
+      </c>
+      <c r="N5" s="6" t="inlineStr">
+        <is>
+          <t>Notification included in CIT return; updated when filing entity changes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
           <t>Germany</t>
         </is>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Conditional</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>Annual</t>
         </is>
       </c>
-      <c r="D5" s="6" t="inlineStr">
+      <c r="D6" s="6" t="inlineStr">
         <is>
           <t>One CE for All</t>
         </is>
       </c>
-      <c r="E5" s="6" t="inlineStr">
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F5" s="6" t="inlineStr">
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G5" s="6" t="inlineStr">
+      <c r="G6" s="6" t="inlineStr">
         <is>
           <t>BZSt Portal</t>
         </is>
       </c>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="H6" s="6" t="inlineStr">
         <is>
           <t>BZSt CbCR Notification</t>
         </is>
       </c>
-      <c r="I5" s="6" t="inlineStr">
+      <c r="I6" s="6" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="J5" s="6" t="inlineStr">
+      <c r="J6" s="6" t="inlineStr">
         <is>
           <t>By end of reporting FY</t>
         </is>
       </c>
-      <c r="K5" s="6" t="inlineStr">
+      <c r="K6" s="6" t="inlineStr">
         <is>
           <t>Annual</t>
         </is>
       </c>
-      <c r="L5" s="6" t="inlineStr">
+      <c r="L6" s="6" t="inlineStr">
         <is>
           <t>CbCR</t>
         </is>
       </c>
-      <c r="M5" s="6" t="inlineStr">
+      <c r="M6" s="6" t="inlineStr">
         <is>
           <t>FY2016</t>
         </is>
       </c>
-      <c r="N5" s="6" t="inlineStr">
+      <c r="N6" s="6" t="inlineStr">
         <is>
           <t>One German group entity can file notification for all German entities</t>
         </is>
@@ -3099,25 +3171,25 @@
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B3:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Always,Conditional,Notification Only,Never Required,N/A"</formula1>
     </dataValidation>
-    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="C3:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Annual,One-Time,Upon Change"</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="D3:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UPE,Local CE,One CE for All,Other"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E3:E1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Yes,No,Not Specified"</formula1>
     </dataValidation>
-    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="F3:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="I3:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"None,CIT Date,FYE-Based,Fixed,Upon Request,With Tax Return"</formula1>
     </dataValidation>
-    <dataValidation sqref="L2:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="L3:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"MF,LF,CbCR,Standalone"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3131,7 +3203,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3221,66 +3293,70 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="6" t="inlineStr">
-        <is>
-          <t>Belgium</t>
-        </is>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Form 275.MF</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>MF Summary</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
-        <is>
-          <t>If MF Required</t>
-        </is>
-      </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t>MF</t>
-        </is>
-      </c>
-      <c r="F2" s="6" t="inlineStr">
-        <is>
-          <t>Summary form with key MF data points</t>
-        </is>
-      </c>
-      <c r="G2" s="6" t="inlineStr">
-        <is>
-          <t>Fixed</t>
-        </is>
-      </c>
-      <c r="H2" s="6" t="inlineStr">
-        <is>
-          <t>31 Dec following FY</t>
-        </is>
-      </c>
-      <c r="I2" s="6" t="inlineStr"/>
-      <c r="J2" s="6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K2" s="6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L2" s="6" t="inlineStr">
-        <is>
-          <t>FY2016</t>
-        </is>
-      </c>
-      <c r="M2" s="6" t="inlineStr">
-        <is>
-          <t>Separate summary form filed alongside full MF report</t>
+    <row r="2" ht="60" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Belgium, Spain, Italy, Germany, etc.</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Form 275.MF / Form 232 / RS 106 / Transaction Matrix</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>TP Disclosure / TP Return / MF Summary / LF Summary / CbCR Notification / Other</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Always / If MF Required / If LF Required / If MF or LF Required / If CbCR Required / Other</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>MF / LF / CbCR / Standalone</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>Summary form with key data / Annual TP informative return / TP disclosure / Structured overview of RPTs</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>None / CIT Date / FYE-Based / Fixed / Upon Request / With Tax Return</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>Details (e.g., 31 Dec following FY, Approx 25 Aug, Within 30 days of audit notice)</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>Days to submit if upon request (30, 14, 10, etc.)</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>Yes / No</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t>Yes / No / Electronic Timestamp</t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>FY2016, 2010, 2024, etc.</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>Context about form requirements and special rules</t>
         </is>
       </c>
     </row>
@@ -3292,37 +3368,37 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>Form 275.LF</t>
+          <t>Form 275.MF</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>LF Summary</t>
+          <t>MF Summary</t>
         </is>
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>If LF Required</t>
+          <t>If MF Required</t>
         </is>
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>LF</t>
+          <t>MF</t>
         </is>
       </c>
       <c r="F3" s="6" t="inlineStr">
         <is>
-          <t>Summary form with key LF data points</t>
+          <t>Summary form with key MF data points</t>
         </is>
       </c>
       <c r="G3" s="6" t="inlineStr">
         <is>
-          <t>With Tax Return</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="H3" s="6" t="inlineStr">
         <is>
-          <t>Expected 31 Jul</t>
+          <t>31 Dec following FY</t>
         </is>
       </c>
       <c r="I3" s="6" t="inlineStr"/>
@@ -3343,49 +3419,49 @@
       </c>
       <c r="M3" s="6" t="inlineStr">
         <is>
-          <t>Separate summary form filed with CIT return</t>
+          <t>Separate summary form filed alongside full MF report</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
-          <t>Form 232</t>
+          <t>Form 275.LF</t>
         </is>
       </c>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>TP Return</t>
+          <t>LF Summary</t>
         </is>
       </c>
       <c r="D4" s="6" t="inlineStr">
         <is>
-          <t>If MF or LF Required</t>
+          <t>If LF Required</t>
         </is>
       </c>
       <c r="E4" s="6" t="inlineStr">
         <is>
-          <t>Standalone</t>
+          <t>LF</t>
         </is>
       </c>
       <c r="F4" s="6" t="inlineStr">
         <is>
-          <t>Annual TP informative return</t>
+          <t>Summary form with key LF data points</t>
         </is>
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>With Tax Return</t>
         </is>
       </c>
       <c r="H4" s="6" t="inlineStr">
         <is>
-          <t>Approx 25 Aug</t>
+          <t>Expected 31 Jul</t>
         </is>
       </c>
       <c r="I4" s="6" t="inlineStr"/>
@@ -3406,24 +3482,24 @@
       </c>
       <c r="M4" s="6" t="inlineStr">
         <is>
-          <t>Informative return separate from full MF/LF documentation</t>
+          <t>Separate summary form filed with CIT return</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>RS 106</t>
+          <t>Form 232</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>TP Disclosure</t>
+          <t>TP Return</t>
         </is>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -3438,17 +3514,17 @@
       </c>
       <c r="F5" s="6" t="inlineStr">
         <is>
-          <t>TP disclosure in tax return</t>
+          <t>Annual TP informative return</t>
         </is>
       </c>
       <c r="G5" s="6" t="inlineStr">
         <is>
-          <t>With Tax Return</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="H5" s="6" t="inlineStr">
         <is>
-          <t>Expected 31 Oct</t>
+          <t>Approx 25 Aug</t>
         </is>
       </c>
       <c r="I5" s="6" t="inlineStr"/>
@@ -3459,80 +3535,143 @@
       </c>
       <c r="K5" s="6" t="inlineStr">
         <is>
-          <t>Electronic Timestamp</t>
+          <t>No</t>
         </is>
       </c>
       <c r="L5" s="6" t="inlineStr">
         <is>
-          <t>FY2010</t>
+          <t>FY2016</t>
         </is>
       </c>
       <c r="M5" s="6" t="inlineStr">
         <is>
-          <t>MF/LF must be electronically timestamped before filing RS 106 disclosure</t>
+          <t>Informative return separate from full MF/LF documentation</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>RS 106</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>TP Disclosure</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>If MF or LF Required</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>Standalone</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>TP disclosure in tax return</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="inlineStr">
+        <is>
+          <t>With Tax Return</t>
+        </is>
+      </c>
+      <c r="H6" s="6" t="inlineStr">
+        <is>
+          <t>Expected 31 Oct</t>
+        </is>
+      </c>
+      <c r="I6" s="6" t="inlineStr"/>
+      <c r="J6" s="6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K6" s="6" t="inlineStr">
+        <is>
+          <t>Electronic Timestamp</t>
+        </is>
+      </c>
+      <c r="L6" s="6" t="inlineStr">
+        <is>
+          <t>FY2010</t>
+        </is>
+      </c>
+      <c r="M6" s="6" t="inlineStr">
+        <is>
+          <t>MF/LF must be electronically timestamped before filing RS 106 disclosure</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
           <t>Germany</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Transaction Matrix</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>TP Disclosure</t>
         </is>
       </c>
-      <c r="D6" s="6" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
         <is>
           <t>Always</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>MF</t>
         </is>
       </c>
-      <c r="F6" s="6" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>Structured overview of RPTs</t>
         </is>
       </c>
-      <c r="G6" s="6" t="inlineStr">
+      <c r="G7" s="6" t="inlineStr">
         <is>
           <t>Upon Request</t>
         </is>
       </c>
-      <c r="H6" s="6" t="inlineStr">
+      <c r="H7" s="6" t="inlineStr">
         <is>
           <t>Within 30 days of audit notice</t>
         </is>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I7" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="J6" s="6" t="inlineStr">
+      <c r="J7" s="6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K6" s="6" t="inlineStr">
+      <c r="K7" s="6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L6" s="6" t="inlineStr">
+      <c r="L7" s="6" t="inlineStr">
         <is>
           <t>FY2024</t>
         </is>
       </c>
-      <c r="M6" s="6" t="inlineStr">
+      <c r="M7" s="6" t="inlineStr">
         <is>
           <t>NEW 2024 requirement - automatic submission with MF upon audit</t>
         </is>
@@ -3540,22 +3679,22 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="C3:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"TP Disclosure,TP Return,MF Summary,LF Summary,CbCR Notification,Other"</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="D3:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Always,If MF Required,If LF Required,If MF or LF Required,If CbCR Required,Other"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E3:E1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"MF,LF,CbCR,Standalone"</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="G3:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"None,CIT Date,FYE-Based,Fixed,Upon Request,With Tax Return"</formula1>
     </dataValidation>
-    <dataValidation sqref="J2:J1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="J3:J1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="K2:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K3:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Yes,No,Electronic Timestamp"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>